<commit_message>
excel stuff coming together
</commit_message>
<xml_diff>
--- a/book/ch4-spreadsheets/res/example1.xlsx
+++ b/book/ch4-spreadsheets/res/example1.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\libraries\Documents\GitHub\computer-apps-primer\ch4-spreadsheets\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\GitHub\computer-apps\book\ch4-spreadsheets\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB9076-9627-423B-8E32-4F2EFB3A4D87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,12 +421,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>